<commit_message>
Implemented modifications for model selection based on validation and train accuracy
</commit_message>
<xml_diff>
--- a/DriverDrowsiness/results/output_base_ff.xlsx
+++ b/DriverDrowsiness/results/output_base_ff.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,30 +491,25 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Test Accuracy</t>
+          <t>Train Accuracy</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
+          <t>Validation Accuracy</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>Model Size</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Recall Drowsy</t>
-        </is>
-      </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Recall Non-Drowsy</t>
+          <t>History Plot</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>History Plot</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Confusion Matrix</t>
         </is>
@@ -571,23 +566,20 @@
         <v>16</v>
       </c>
       <c r="L2" t="n">
-        <v>87.00000047683716</v>
+        <v>1</v>
       </c>
       <c r="M2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" t="n">
         <v>189.1264686584473</v>
       </c>
-      <c r="N2" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0.78</v>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>./plots/base_full_face/hist/history_1.png</t>
+        </is>
       </c>
       <c r="P2" t="inlineStr">
-        <is>
-          <t>./plots/base_full_face/hist/history_1.png</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
         <is>
           <t>./plots/base_full_face/cm/confusion_matrix_1.png</t>
         </is>
@@ -644,23 +636,20 @@
         <v>16</v>
       </c>
       <c r="L3" t="n">
-        <v>79.00000214576721</v>
+        <v>1</v>
       </c>
       <c r="M3" t="n">
+        <v>0.9666666388511658</v>
+      </c>
+      <c r="N3" t="n">
         <v>189.1264686584473</v>
       </c>
-      <c r="N3" t="n">
-        <v>0.74</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0.82</v>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>./plots/base_full_face/hist/history_2.png</t>
+        </is>
       </c>
       <c r="P3" t="inlineStr">
-        <is>
-          <t>./plots/base_full_face/hist/history_2.png</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
         <is>
           <t>./plots/base_full_face/cm/confusion_matrix_2.png</t>
         </is>
@@ -717,23 +706,20 @@
         <v>16</v>
       </c>
       <c r="L4" t="n">
-        <v>75.99999904632568</v>
+        <v>1</v>
       </c>
       <c r="M4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" t="n">
         <v>126.5555458068848</v>
       </c>
-      <c r="N4" t="n">
-        <v>0.86</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0.6</v>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>./plots/base_full_face/hist/history_3.png</t>
+        </is>
       </c>
       <c r="P4" t="inlineStr">
-        <is>
-          <t>./plots/base_full_face/hist/history_3.png</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
         <is>
           <t>./plots/base_full_face/cm/confusion_matrix_3.png</t>
         </is>
@@ -790,23 +776,20 @@
         <v>16</v>
       </c>
       <c r="L5" t="n">
-        <v>73.00000190734863</v>
+        <v>1</v>
       </c>
       <c r="M5" t="n">
+        <v>0.9833333492279053</v>
+      </c>
+      <c r="N5" t="n">
         <v>126.5555458068848</v>
       </c>
-      <c r="N5" t="n">
-        <v>0.82</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0.5600000000000001</v>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>./plots/base_full_face/hist/history_4.png</t>
+        </is>
       </c>
       <c r="P5" t="inlineStr">
-        <is>
-          <t>./plots/base_full_face/hist/history_4.png</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
         <is>
           <t>./plots/base_full_face/cm/confusion_matrix_4.png</t>
         </is>
@@ -863,23 +846,20 @@
         <v>16</v>
       </c>
       <c r="L6" t="n">
-        <v>69.9999988079071</v>
+        <v>1</v>
       </c>
       <c r="M6" t="n">
+        <v>0.9833333492279053</v>
+      </c>
+      <c r="N6" t="n">
         <v>151.3449745178223</v>
       </c>
-      <c r="N6" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0.48</v>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>./plots/base_full_face/hist/history_5.png</t>
+        </is>
       </c>
       <c r="P6" t="inlineStr">
-        <is>
-          <t>./plots/base_full_face/hist/history_5.png</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
         <is>
           <t>./plots/base_full_face/cm/confusion_matrix_5.png</t>
         </is>
@@ -936,23 +916,20 @@
         <v>16</v>
       </c>
       <c r="L7" t="n">
-        <v>81.00000023841858</v>
+        <v>1</v>
       </c>
       <c r="M7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N7" t="n">
         <v>151.3449745178223</v>
       </c>
-      <c r="N7" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0.86</v>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>./plots/base_full_face/hist/history_6.png</t>
+        </is>
       </c>
       <c r="P7" t="inlineStr">
-        <is>
-          <t>./plots/base_full_face/hist/history_6.png</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
         <is>
           <t>./plots/base_full_face/cm/confusion_matrix_6.png</t>
         </is>
@@ -1009,23 +986,20 @@
         <v>16</v>
       </c>
       <c r="L8" t="n">
-        <v>74.00000095367432</v>
+        <v>1</v>
       </c>
       <c r="M8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" t="n">
         <v>101.2740516662598</v>
       </c>
-      <c r="N8" t="n">
-        <v>0.88</v>
-      </c>
-      <c r="O8" t="n">
-        <v>0.6</v>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>./plots/base_full_face/hist/history_7.png</t>
+        </is>
       </c>
       <c r="P8" t="inlineStr">
-        <is>
-          <t>./plots/base_full_face/hist/history_7.png</t>
-        </is>
-      </c>
-      <c r="Q8" t="inlineStr">
         <is>
           <t>./plots/base_full_face/cm/confusion_matrix_7.png</t>
         </is>
@@ -1082,23 +1056,20 @@
         <v>16</v>
       </c>
       <c r="L9" t="n">
-        <v>68.99999976158142</v>
+        <v>1</v>
       </c>
       <c r="M9" t="n">
+        <v>0.9833333492279053</v>
+      </c>
+      <c r="N9" t="n">
         <v>101.2740516662598</v>
       </c>
-      <c r="N9" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="O9" t="n">
-        <v>0.46</v>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>./plots/base_full_face/hist/history_8.png</t>
+        </is>
       </c>
       <c r="P9" t="inlineStr">
-        <is>
-          <t>./plots/base_full_face/hist/history_8.png</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
         <is>
           <t>./plots/base_full_face/cm/confusion_matrix_8.png</t>
         </is>

</xml_diff>

<commit_message>
Intermediate version of notebook with recall analysis. Partially complete
</commit_message>
<xml_diff>
--- a/DriverDrowsiness/results/output_base_ff.xlsx
+++ b/DriverDrowsiness/results/output_base_ff.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,15 +501,40 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
+          <t>Test Accuracy</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>Model Size</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Train Recall</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Val Recall</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Drowsy Recall</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Non-Drowsy Recall</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>History Plot</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Confusion Matrix</t>
         </is>
@@ -566,20 +591,35 @@
         <v>16</v>
       </c>
       <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>81.99999928474426</v>
+      </c>
+      <c r="O2" t="n">
+        <v>189.1264686584473</v>
+      </c>
+      <c r="P2" t="n">
         <v>1</v>
       </c>
-      <c r="M2" t="n">
-        <v>1</v>
-      </c>
-      <c r="N2" t="n">
-        <v>189.1264686584473</v>
-      </c>
-      <c r="O2" t="inlineStr">
+      <c r="Q2" t="n">
+        <v>0.96875</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="T2" t="inlineStr">
         <is>
           <t>./plots/base_full_face/hist/history_1.png</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>./plots/base_full_face/cm/confusion_matrix_1.png</t>
         </is>
@@ -636,20 +676,35 @@
         <v>16</v>
       </c>
       <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>80.0000011920929</v>
+      </c>
+      <c r="O3" t="n">
+        <v>189.1264686584473</v>
+      </c>
+      <c r="P3" t="n">
         <v>1</v>
       </c>
-      <c r="M3" t="n">
-        <v>0.9666666388511658</v>
-      </c>
-      <c r="N3" t="n">
-        <v>189.1264686584473</v>
-      </c>
-      <c r="O3" t="inlineStr">
+      <c r="Q3" t="n">
+        <v>0.96875</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="T3" t="inlineStr">
         <is>
           <t>./plots/base_full_face/hist/history_2.png</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="U3" t="inlineStr">
         <is>
           <t>./plots/base_full_face/cm/confusion_matrix_2.png</t>
         </is>
@@ -706,20 +761,35 @@
         <v>16</v>
       </c>
       <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>83.99999737739563</v>
+      </c>
+      <c r="O4" t="n">
+        <v>126.5555458068848</v>
+      </c>
+      <c r="P4" t="n">
         <v>1</v>
       </c>
-      <c r="M4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N4" t="n">
-        <v>126.5555458068848</v>
-      </c>
-      <c r="O4" t="inlineStr">
+      <c r="Q4" t="n">
+        <v>0.96875</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="T4" t="inlineStr">
         <is>
           <t>./plots/base_full_face/hist/history_3.png</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="U4" t="inlineStr">
         <is>
           <t>./plots/base_full_face/cm/confusion_matrix_3.png</t>
         </is>
@@ -776,20 +846,35 @@
         <v>16</v>
       </c>
       <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>77.99999713897705</v>
+      </c>
+      <c r="O5" t="n">
+        <v>126.5555458068848</v>
+      </c>
+      <c r="P5" t="n">
         <v>1</v>
       </c>
-      <c r="M5" t="n">
-        <v>0.9833333492279053</v>
-      </c>
-      <c r="N5" t="n">
-        <v>126.5555458068848</v>
-      </c>
-      <c r="O5" t="inlineStr">
+      <c r="Q5" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="T5" t="inlineStr">
         <is>
           <t>./plots/base_full_face/hist/history_4.png</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="U5" t="inlineStr">
         <is>
           <t>./plots/base_full_face/cm/confusion_matrix_4.png</t>
         </is>
@@ -846,20 +931,35 @@
         <v>16</v>
       </c>
       <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>83.99999737739563</v>
+      </c>
+      <c r="O6" t="n">
+        <v>151.3449745178223</v>
+      </c>
+      <c r="P6" t="n">
         <v>1</v>
       </c>
-      <c r="M6" t="n">
-        <v>0.9833333492279053</v>
-      </c>
-      <c r="N6" t="n">
-        <v>151.3449745178223</v>
-      </c>
-      <c r="O6" t="inlineStr">
+      <c r="Q6" t="n">
+        <v>1</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="T6" t="inlineStr">
         <is>
           <t>./plots/base_full_face/hist/history_5.png</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
+      <c r="U6" t="inlineStr">
         <is>
           <t>./plots/base_full_face/cm/confusion_matrix_5.png</t>
         </is>
@@ -916,20 +1016,35 @@
         <v>16</v>
       </c>
       <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>95.99999785423279</v>
+      </c>
+      <c r="O7" t="n">
+        <v>151.3449745178223</v>
+      </c>
+      <c r="P7" t="n">
         <v>1</v>
       </c>
-      <c r="M7" t="n">
+      <c r="Q7" t="n">
         <v>1</v>
       </c>
-      <c r="N7" t="n">
-        <v>151.3449745178223</v>
-      </c>
-      <c r="O7" t="inlineStr">
+      <c r="R7" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="T7" t="inlineStr">
         <is>
           <t>./plots/base_full_face/hist/history_6.png</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr">
+      <c r="U7" t="inlineStr">
         <is>
           <t>./plots/base_full_face/cm/confusion_matrix_6.png</t>
         </is>
@@ -986,20 +1101,35 @@
         <v>16</v>
       </c>
       <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>92.00000166893005</v>
+      </c>
+      <c r="O8" t="n">
+        <v>101.2740516662598</v>
+      </c>
+      <c r="P8" t="n">
         <v>1</v>
       </c>
-      <c r="M8" t="n">
-        <v>1</v>
-      </c>
-      <c r="N8" t="n">
-        <v>101.2740516662598</v>
-      </c>
-      <c r="O8" t="inlineStr">
+      <c r="Q8" t="n">
+        <v>0.9375</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="T8" t="inlineStr">
         <is>
           <t>./plots/base_full_face/hist/history_7.png</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr">
+      <c r="U8" t="inlineStr">
         <is>
           <t>./plots/base_full_face/cm/confusion_matrix_7.png</t>
         </is>
@@ -1056,20 +1186,35 @@
         <v>16</v>
       </c>
       <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>66.00000262260437</v>
+      </c>
+      <c r="O9" t="n">
+        <v>101.2740516662598</v>
+      </c>
+      <c r="P9" t="n">
         <v>1</v>
       </c>
-      <c r="M9" t="n">
-        <v>0.9833333492279053</v>
-      </c>
-      <c r="N9" t="n">
-        <v>101.2740516662598</v>
-      </c>
-      <c r="O9" t="inlineStr">
+      <c r="Q9" t="n">
+        <v>0.96875</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="T9" t="inlineStr">
         <is>
           <t>./plots/base_full_face/hist/history_8.png</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
+      <c r="U9" t="inlineStr">
         <is>
           <t>./plots/base_full_face/cm/confusion_matrix_8.png</t>
         </is>

</xml_diff>

<commit_message>
Final Code Update Checkin For 207 Project
</commit_message>
<xml_diff>
--- a/DriverDrowsiness/results/output_base_ff.xlsx
+++ b/DriverDrowsiness/results/output_base_ff.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,42 +501,12 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Test Accuracy</t>
+          <t>Model Size</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Model Size</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Train Recall</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Val Recall</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Drowsy Recall</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Non-Drowsy Recall</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
           <t>History Plot</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Confusion Matrix</t>
         </is>
       </c>
     </row>
@@ -591,37 +561,17 @@
         <v>16</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N2" t="n">
-        <v>81.99999928474426</v>
-      </c>
-      <c r="O2" t="n">
         <v>189.1264686584473</v>
       </c>
-      <c r="P2" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>0.96875</v>
-      </c>
-      <c r="R2" t="n">
-        <v>0.88</v>
-      </c>
-      <c r="S2" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>./plots/base_full_face/hist/history_1.png</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>./plots/base_full_face/cm/confusion_matrix_1.png</t>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>./plots/base_full_face/hist/history_0.png</t>
         </is>
       </c>
     </row>
@@ -676,37 +626,17 @@
         <v>16</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3" t="n">
-        <v>80.0000011920929</v>
-      </c>
-      <c r="O3" t="n">
         <v>189.1264686584473</v>
       </c>
-      <c r="P3" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0.96875</v>
-      </c>
-      <c r="R3" t="n">
-        <v>0.84</v>
-      </c>
-      <c r="S3" t="n">
-        <v>0.62</v>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>./plots/base_full_face/hist/history_2.png</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>./plots/base_full_face/cm/confusion_matrix_2.png</t>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>./plots/base_full_face/hist/history_1.png</t>
         </is>
       </c>
     </row>
@@ -761,37 +691,17 @@
         <v>16</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>0.949999988079071</v>
       </c>
       <c r="N4" t="n">
-        <v>83.99999737739563</v>
-      </c>
-      <c r="O4" t="n">
         <v>126.5555458068848</v>
       </c>
-      <c r="P4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>0.96875</v>
-      </c>
-      <c r="R4" t="n">
-        <v>0.86</v>
-      </c>
-      <c r="S4" t="n">
-        <v>0.64</v>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>./plots/base_full_face/hist/history_3.png</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>./plots/base_full_face/cm/confusion_matrix_3.png</t>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>./plots/base_full_face/hist/history_2.png</t>
         </is>
       </c>
     </row>
@@ -846,37 +756,17 @@
         <v>16</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>0.9833333492279053</v>
       </c>
       <c r="N5" t="n">
-        <v>77.99999713897705</v>
-      </c>
-      <c r="O5" t="n">
         <v>126.5555458068848</v>
       </c>
-      <c r="P5" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>1</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="S5" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>./plots/base_full_face/hist/history_4.png</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>./plots/base_full_face/cm/confusion_matrix_4.png</t>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>./plots/base_full_face/hist/history_3.png</t>
         </is>
       </c>
     </row>
@@ -931,37 +821,17 @@
         <v>16</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>0.9833333492279053</v>
       </c>
       <c r="N6" t="n">
-        <v>83.99999737739563</v>
-      </c>
-      <c r="O6" t="n">
         <v>151.3449745178223</v>
       </c>
-      <c r="P6" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>1</v>
-      </c>
-      <c r="R6" t="n">
-        <v>0.88</v>
-      </c>
-      <c r="S6" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>./plots/base_full_face/hist/history_5.png</t>
-        </is>
-      </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>./plots/base_full_face/cm/confusion_matrix_5.png</t>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>./plots/base_full_face/hist/history_4.png</t>
         </is>
       </c>
     </row>
@@ -1016,37 +886,17 @@
         <v>16</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" t="n">
-        <v>95.99999785423279</v>
-      </c>
-      <c r="O7" t="n">
         <v>151.3449745178223</v>
       </c>
-      <c r="P7" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>1</v>
-      </c>
-      <c r="R7" t="n">
-        <v>0.98</v>
-      </c>
-      <c r="S7" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>./plots/base_full_face/hist/history_6.png</t>
-        </is>
-      </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>./plots/base_full_face/cm/confusion_matrix_6.png</t>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>./plots/base_full_face/hist/history_5.png</t>
         </is>
       </c>
     </row>
@@ -1101,37 +951,17 @@
         <v>16</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>0.9937499761581421</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8" t="n">
-        <v>92.00000166893005</v>
-      </c>
-      <c r="O8" t="n">
         <v>101.2740516662598</v>
       </c>
-      <c r="P8" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>0.9375</v>
-      </c>
-      <c r="R8" t="n">
-        <v>0.96</v>
-      </c>
-      <c r="S8" t="n">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="T8" t="inlineStr">
-        <is>
-          <t>./plots/base_full_face/hist/history_7.png</t>
-        </is>
-      </c>
-      <c r="U8" t="inlineStr">
-        <is>
-          <t>./plots/base_full_face/cm/confusion_matrix_7.png</t>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>./plots/base_full_face/hist/history_6.png</t>
         </is>
       </c>
     </row>
@@ -1186,37 +1016,17 @@
         <v>16</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9" t="n">
-        <v>66.00000262260437</v>
-      </c>
-      <c r="O9" t="n">
         <v>101.2740516662598</v>
       </c>
-      <c r="P9" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>0.96875</v>
-      </c>
-      <c r="R9" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="S9" t="n">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="T9" t="inlineStr">
-        <is>
-          <t>./plots/base_full_face/hist/history_8.png</t>
-        </is>
-      </c>
-      <c r="U9" t="inlineStr">
-        <is>
-          <t>./plots/base_full_face/cm/confusion_matrix_8.png</t>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>./plots/base_full_face/hist/history_7.png</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated model run for baseline
</commit_message>
<xml_diff>
--- a/DriverDrowsiness/results/output_base_ff.xlsx
+++ b/DriverDrowsiness/results/output_base_ff.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[(3, 3), (3, 3)]</t>
+          <t>[(3, 3), (3, 3), (3, 3)]</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -564,7 +564,7 @@
         <v>1</v>
       </c>
       <c r="M2" t="n">
-        <v>1</v>
+        <v>0.9833333492279053</v>
       </c>
       <c r="N2" t="n">
         <v>189.1264686584473</v>
@@ -586,7 +586,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>[(3, 3), (3, 3)]</t>
+          <t>[(3, 3), (3, 3), (3, 3)]</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -651,7 +651,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>[(3, 3), (3, 3)]</t>
+          <t>[(3, 3), (3, 3), (3, 3)]</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -694,7 +694,7 @@
         <v>1</v>
       </c>
       <c r="M4" t="n">
-        <v>0.949999988079071</v>
+        <v>0.9833333492279053</v>
       </c>
       <c r="N4" t="n">
         <v>126.5555458068848</v>
@@ -716,7 +716,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>[(3, 3), (3, 3)]</t>
+          <t>[(3, 3), (3, 3), (3, 3)]</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>[(3, 3), (3, 3)]</t>
+          <t>[(3, 3), (3, 3), (3, 3)]</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -821,10 +821,10 @@
         <v>16</v>
       </c>
       <c r="L6" t="n">
+        <v>0.9937499761581421</v>
+      </c>
+      <c r="M6" t="n">
         <v>1</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.9833333492279053</v>
       </c>
       <c r="N6" t="n">
         <v>151.3449745178223</v>
@@ -846,7 +846,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>[(3, 3), (3, 3)]</t>
+          <t>[(3, 3), (3, 3), (3, 3)]</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -889,7 +889,7 @@
         <v>1</v>
       </c>
       <c r="M7" t="n">
-        <v>1</v>
+        <v>0.949999988079071</v>
       </c>
       <c r="N7" t="n">
         <v>151.3449745178223</v>
@@ -911,7 +911,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>[(3, 3), (3, 3)]</t>
+          <t>[(3, 3), (3, 3), (3, 3)]</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -951,10 +951,10 @@
         <v>16</v>
       </c>
       <c r="L8" t="n">
-        <v>0.9937499761581421</v>
+        <v>0.9916666746139526</v>
       </c>
       <c r="M8" t="n">
-        <v>1</v>
+        <v>0.9333333373069763</v>
       </c>
       <c r="N8" t="n">
         <v>101.2740516662598</v>
@@ -976,7 +976,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>[(3, 3), (3, 3)]</t>
+          <t>[(3, 3), (3, 3), (3, 3)]</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">

</xml_diff>